<commit_message>
Hay que corregir las validaciones del Login
</commit_message>
<xml_diff>
--- a/registros.xlsx
+++ b/registros.xlsx
@@ -434,7 +434,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -443,7 +443,7 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="12" customWidth="1" min="1" max="1"/>
-    <col width="8" customWidth="1" min="2" max="2"/>
+    <col width="12" customWidth="1" min="2" max="2"/>
     <col width="12" customWidth="1" min="3" max="3"/>
   </cols>
   <sheetData>
@@ -517,19 +517,45 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>1025896631</t>
-        </is>
+      <c r="A6" t="n">
+        <v>1025896631</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
           <t>Hola</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>5051680725</t>
+      <c r="C6" t="n">
+        <v>5051680725</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>1000535410</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>alberto</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>3245619850</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>1017237015</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Estefania </t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>3057897240</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Cambios a Gestion de clientes, se removio la tabla de eliminar cliente y se añadieron ventanas de aviso para la añadición de clientes
</commit_message>
<xml_diff>
--- a/registros.xlsx
+++ b/registros.xlsx
@@ -434,7 +434,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -443,7 +443,7 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="12" customWidth="1" min="1" max="1"/>
-    <col width="12" customWidth="1" min="2" max="2"/>
+    <col width="19" customWidth="1" min="2" max="2"/>
     <col width="12" customWidth="1" min="3" max="3"/>
   </cols>
   <sheetData>
@@ -543,20 +543,55 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>1017237015</t>
-        </is>
+      <c r="A8" t="n">
+        <v>1017237015</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
           <t xml:space="preserve">Estefania </t>
         </is>
       </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>3057897240</t>
-        </is>
+      <c r="C8" t="n">
+        <v>3057897240</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>4848484848</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>asdasdasdasdasdas</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>1234567890</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>1234567891</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Pedro</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>3014386600</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>1234567891</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>aaaa</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>3245619850</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Se arreglo el login
</commit_message>
<xml_diff>
--- a/registros.xlsx
+++ b/registros.xlsx
@@ -434,7 +434,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -444,7 +444,7 @@
   <cols>
     <col width="12" customWidth="1" min="1" max="1"/>
     <col width="8" customWidth="1" min="2" max="2"/>
-    <col width="12" customWidth="1" min="3" max="3"/>
+    <col width="10" customWidth="1" min="3" max="3"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -465,71 +465,19 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
-        <v>103318341</v>
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>1034918141</t>
+        </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Juan</t>
-        </is>
-      </c>
-      <c r="C2" t="n">
-        <v>3052076540</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>1034918141</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
           <t>Daniel</t>
         </is>
       </c>
-      <c r="C3" t="n">
-        <v>3052076540</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>103781841</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Daniel</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
-        <v>3086547892</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>103781841</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Daniel</t>
-        </is>
-      </c>
-      <c r="C5" t="n">
-        <v>3086547892</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>1025896631</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Hola</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>5051680725</t>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>50516800</t>
         </is>
       </c>
     </row>
@@ -1081,8 +1029,10 @@
           <t>soporte</t>
         </is>
       </c>
-      <c r="C2" t="n">
-        <v>123</v>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>hola</t>
+        </is>
       </c>
       <c r="D2" t="n">
         <v>1</v>

</xml_diff>

<commit_message>
cambios a gestion servicios ui
</commit_message>
<xml_diff>
--- a/registros.xlsx
+++ b/registros.xlsx
@@ -434,7 +434,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -592,6 +592,32 @@
       </c>
       <c r="C11" t="n">
         <v>3245619850</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>1000535410</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>sdafsafdsdf</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>6648792520</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>1000535410</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>aasd</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>2269735498</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
funciona el login, hay que completa la gestion de servicios y cliente
</commit_message>
<xml_diff>
--- a/registros.xlsx
+++ b/registros.xlsx
@@ -434,7 +434,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -442,8 +442,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="12" customWidth="1" min="1" max="1"/>
-    <col width="19" customWidth="1" min="2" max="2"/>
+    <col width="11" customWidth="1" min="1" max="1"/>
+    <col width="8" customWidth="1" min="2" max="2"/>
     <col width="12" customWidth="1" min="3" max="3"/>
   </cols>
   <sheetData>
@@ -479,7 +479,7 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>1034918141</v>
+        <v>103491814</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
@@ -488,136 +488,6 @@
       </c>
       <c r="C3" t="n">
         <v>3052076540</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>103781841</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Daniel</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
-        <v>3086547892</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>103781841</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Daniel</t>
-        </is>
-      </c>
-      <c r="C5" t="n">
-        <v>3086547892</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>1025896631</v>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Hola</t>
-        </is>
-      </c>
-      <c r="C6" t="n">
-        <v>5051680725</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>1000535410</v>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>alberto</t>
-        </is>
-      </c>
-      <c r="C7" t="n">
-        <v>3245619850</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>1017237015</v>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Estefania </t>
-        </is>
-      </c>
-      <c r="C8" t="n">
-        <v>3057897240</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="n">
-        <v>4848484848</v>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>asdasdasdasdasdas</t>
-        </is>
-      </c>
-      <c r="C9" t="n">
-        <v>1234567890</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="n">
-        <v>1234567891</v>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>Pedro</t>
-        </is>
-      </c>
-      <c r="C10" t="n">
-        <v>3014386600</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="n">
-        <v>1234567891</v>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>aaaa</t>
-        </is>
-      </c>
-      <c r="C11" t="n">
-        <v>3245619850</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="n">
-        <v>1000535410</v>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>sdafsafdsdf</t>
-        </is>
-      </c>
-      <c r="C12" t="n">
-        <v>6648792520</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="n">
-        <v>1000535410</v>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>aasd</t>
-        </is>
-      </c>
-      <c r="C13" t="n">
-        <v>2269735498</v>
       </c>
     </row>
   </sheetData>
@@ -1123,7 +993,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1168,11 +1038,49 @@
           <t>soporte</t>
         </is>
       </c>
-      <c r="C2" t="n">
-        <v>123</v>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>hola</t>
+        </is>
       </c>
       <c r="D2" t="n">
         <v>1</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>cajero</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>cajero</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>admin</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>admin</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
La parte de gestion clientes en diseño esta terminasa, solo falta validar algunos campos y comprobar el error al tratar de eliminar los datos
</commit_message>
<xml_diff>
--- a/registros.xlsx
+++ b/registros.xlsx
@@ -434,7 +434,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -442,9 +442,9 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="11" customWidth="1" min="1" max="1"/>
-    <col width="8" customWidth="1" min="2" max="2"/>
-    <col width="12" customWidth="1" min="3" max="3"/>
+    <col width="12" customWidth="1" min="1" max="1"/>
+    <col width="18" customWidth="1" min="2" max="2"/>
+    <col width="10" customWidth="1" min="3" max="3"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -466,28 +466,15 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>103318341</v>
+        <v>9332945823</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Juan</t>
+          <t>pedro picapiedra</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>3052076540</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>103491814</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Daniel</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
-        <v>3052076540</v>
+        <v>22691392</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
solucion a a la conexion con la base de datos
</commit_message>
<xml_diff>
--- a/registros.xlsx
+++ b/registros.xlsx
@@ -442,9 +442,9 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="13" customWidth="1" min="1" max="1"/>
-    <col width="8" customWidth="1" min="2" max="2"/>
-    <col width="11" customWidth="1" min="3" max="3"/>
+    <col width="11" customWidth="1" min="1" max="1"/>
+    <col width="17" customWidth="1" min="2" max="2"/>
+    <col width="12" customWidth="1" min="3" max="3"/>
     <col width="8" customWidth="1" min="4" max="4"/>
   </cols>
   <sheetData>
@@ -472,18 +472,15 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>12131313313</v>
+        <v>901234359</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t xml:space="preserve">Goofy </t>
+          <t>Pedro la piedra</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>324560234</v>
-      </c>
-      <c r="D2" t="b">
-        <v>1</v>
+        <v>3453682345</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
metodo de base de datos para validar si la venta es servicio, producto o ambas
</commit_message>
<xml_diff>
--- a/registros.xlsx
+++ b/registros.xlsx
@@ -442,9 +442,9 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="11" customWidth="1" min="1" max="1"/>
-    <col width="11" customWidth="1" min="2" max="2"/>
-    <col width="17" customWidth="1" min="3" max="3"/>
+    <col width="12" customWidth="1" min="1" max="1"/>
+    <col width="18" customWidth="1" min="2" max="2"/>
+    <col width="12" customWidth="1" min="3" max="3"/>
     <col width="8" customWidth="1" min="4" max="4"/>
   </cols>
   <sheetData>
@@ -472,17 +472,15 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>901234354</v>
+        <v>1000545230</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>La piedra</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>effdsfsdfsdfsfd</t>
-        </is>
+          <t>Baltazar Sanchez</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>4325465745</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
validaciones minimas culminadas en reportes y cambiar contraseña
</commit_message>
<xml_diff>
--- a/registros.xlsx
+++ b/registros.xlsx
@@ -434,7 +434,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -442,10 +442,9 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="12" customWidth="1" min="1" max="1"/>
-    <col width="18" customWidth="1" min="2" max="2"/>
-    <col width="12" customWidth="1" min="3" max="3"/>
-    <col width="8" customWidth="1" min="4" max="4"/>
+    <col width="8" customWidth="1" min="1" max="1"/>
+    <col width="8" customWidth="1" min="2" max="2"/>
+    <col width="10" customWidth="1" min="3" max="3"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -463,24 +462,6 @@
         <is>
           <t>Telefono</t>
         </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Activo</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="n">
-        <v>1000545230</v>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Baltazar Sanchez</t>
-        </is>
-      </c>
-      <c r="C2" t="n">
-        <v>4325465745</v>
       </c>
     </row>
   </sheetData>
@@ -559,7 +540,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -569,12 +550,12 @@
   <cols>
     <col width="12" customWidth="1" min="1" max="1"/>
     <col width="18" customWidth="1" min="2" max="2"/>
-    <col width="8" customWidth="1" min="3" max="3"/>
+    <col width="7" customWidth="1" min="3" max="3"/>
     <col width="23" customWidth="1" min="4" max="4"/>
     <col width="14" customWidth="1" min="5" max="5"/>
     <col width="19" customWidth="1" min="6" max="6"/>
     <col width="21" customWidth="1" min="7" max="7"/>
-    <col width="18" customWidth="1" min="8" max="8"/>
+    <col width="7" customWidth="1" min="8" max="8"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -616,230 +597,6 @@
       <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Fecha</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Labial</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
-        <v>1234579114328</v>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Avon</t>
-        </is>
-      </c>
-      <c r="D2" t="n">
-        <v>6000</v>
-      </c>
-      <c r="E2" t="n">
-        <v>10000</v>
-      </c>
-      <c r="F2" t="n">
-        <v>5</v>
-      </c>
-      <c r="G2" t="b">
-        <v>1</v>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>02/06/2024 17:52</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Dea</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
-        <v>1234579114330</v>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>asad</t>
-        </is>
-      </c>
-      <c r="D3" t="n">
-        <v>1234</v>
-      </c>
-      <c r="E3" t="n">
-        <v>1234</v>
-      </c>
-      <c r="F3" t="n">
-        <v>4</v>
-      </c>
-      <c r="G3" t="b">
-        <v>1</v>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>02/06/2024 17:59</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>aaa</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
-        <v>1234567890123</v>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>vbbbb</t>
-        </is>
-      </c>
-      <c r="D4" t="n">
-        <v>30000</v>
-      </c>
-      <c r="E4" t="n">
-        <v>100000</v>
-      </c>
-      <c r="F4" t="n">
-        <v>9</v>
-      </c>
-      <c r="G4" t="b">
-        <v>1</v>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>02/06/2024 18:02</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>111</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>1234567890123</v>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Da</t>
-        </is>
-      </c>
-      <c r="D5" t="n">
-        <v>23</v>
-      </c>
-      <c r="E5" t="n">
-        <v>362</v>
-      </c>
-      <c r="F5" t="n">
-        <v>6</v>
-      </c>
-      <c r="G5" t="b">
-        <v>1</v>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>02/06/2024 18:24</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>PapaWlol</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
-        <v>4234254353243</v>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Frisby</t>
-        </is>
-      </c>
-      <c r="D6" t="n">
-        <v>5000</v>
-      </c>
-      <c r="E6" t="n">
-        <v>80000</v>
-      </c>
-      <c r="F6" t="n">
-        <v>900</v>
-      </c>
-      <c r="G6" t="b">
-        <v>1</v>
-      </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>03/06/2024 18:52</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>Zapatoss</t>
-        </is>
-      </c>
-      <c r="B7" t="n">
-        <v>7788996677886</v>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>Nike</t>
-        </is>
-      </c>
-      <c r="D7" t="n">
-        <v>400000</v>
-      </c>
-      <c r="E7" t="n">
-        <v>800000</v>
-      </c>
-      <c r="F7" t="n">
-        <v>69</v>
-      </c>
-      <c r="G7" t="b">
-        <v>1</v>
-      </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>03/06/2024 19:01</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>Pcs</t>
-        </is>
-      </c>
-      <c r="B8" t="n">
-        <v>4038408439030</v>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>Lapsus</t>
-        </is>
-      </c>
-      <c r="D8" t="n">
-        <v>9888000</v>
-      </c>
-      <c r="E8" t="n">
-        <v>388888888</v>
-      </c>
-      <c r="F8" t="n">
-        <v>89898</v>
-      </c>
-      <c r="G8" t="b">
-        <v>1</v>
-      </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>03/06/2024 19:10</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
los tipos de datos estan afectando todo pa, terrible.
</commit_message>
<xml_diff>
--- a/registros.xlsx
+++ b/registros.xlsx
@@ -434,7 +434,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -481,6 +481,45 @@
       </c>
       <c r="C2" t="n">
         <v>4325465745</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>1000535410</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Albeiro Molina</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>3245619849</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>1888473247</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Pedro la piedra</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>2342345467</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>1222323423</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Validasras</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>323234323</v>
       </c>
     </row>
   </sheetData>
@@ -559,7 +598,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -569,7 +608,7 @@
   <cols>
     <col width="12" customWidth="1" min="1" max="1"/>
     <col width="18" customWidth="1" min="2" max="2"/>
-    <col width="8" customWidth="1" min="3" max="3"/>
+    <col width="9" customWidth="1" min="3" max="3"/>
     <col width="23" customWidth="1" min="4" max="4"/>
     <col width="14" customWidth="1" min="5" max="5"/>
     <col width="19" customWidth="1" min="6" max="6"/>
@@ -840,6 +879,166 @@
       <c r="H8" t="inlineStr">
         <is>
           <t>03/06/2024 19:10</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>asdfsdfa</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>2423423423423</v>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>sfsfsdf</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>324234</v>
+      </c>
+      <c r="E9" t="n">
+        <v>324234</v>
+      </c>
+      <c r="F9" t="n">
+        <v>234234</v>
+      </c>
+      <c r="G9" t="b">
+        <v>1</v>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>04/06/2024 02:49</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>edadasdad</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>2313131232131</v>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>fafasf</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>223423</v>
+      </c>
+      <c r="E10" t="n">
+        <v>223434</v>
+      </c>
+      <c r="F10" t="n">
+        <v>232423</v>
+      </c>
+      <c r="G10" t="b">
+        <v>1</v>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>04/06/2024 03:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>dsfsdf</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>2313131232133</v>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>fafasf</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>223423</v>
+      </c>
+      <c r="E11" t="n">
+        <v>223434</v>
+      </c>
+      <c r="F11" t="n">
+        <v>232423</v>
+      </c>
+      <c r="G11" t="b">
+        <v>1</v>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>04/06/2024 03:02</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>teclados</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>3245234543252</v>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Basura</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>34252</v>
+      </c>
+      <c r="E12" t="n">
+        <v>324534</v>
+      </c>
+      <c r="F12" t="n">
+        <v>245234</v>
+      </c>
+      <c r="G12" t="b">
+        <v>1</v>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>04/06/2024 04:44</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>sfdsfafa</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>2342342343242</v>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>wqqtrre</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>23424</v>
+      </c>
+      <c r="E13" t="n">
+        <v>3424234</v>
+      </c>
+      <c r="F13" t="n">
+        <v>2342342</v>
+      </c>
+      <c r="G13" t="b">
+        <v>1</v>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>04/06/2024 04:46</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Se arreglo la validacion de modificar productos.
</commit_message>
<xml_diff>
--- a/registros.xlsx
+++ b/registros.xlsx
@@ -598,7 +598,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -606,9 +606,9 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="12" customWidth="1" min="1" max="1"/>
+    <col width="13" customWidth="1" min="1" max="1"/>
     <col width="18" customWidth="1" min="2" max="2"/>
-    <col width="9" customWidth="1" min="3" max="3"/>
+    <col width="11" customWidth="1" min="3" max="3"/>
     <col width="23" customWidth="1" min="4" max="4"/>
     <col width="14" customWidth="1" min="5" max="5"/>
     <col width="19" customWidth="1" min="6" max="6"/>
@@ -669,14 +669,14 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Avon</t>
+          <t>sdfsdfs</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>6000</v>
+        <v>4234</v>
       </c>
       <c r="E2" t="n">
-        <v>10000</v>
+        <v>2342</v>
       </c>
       <c r="F2" t="n">
         <v>5</v>
@@ -957,14 +957,14 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>fafasf</t>
+          <t>fsdffsf</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>223423</v>
+        <v>234234</v>
       </c>
       <c r="E11" t="n">
-        <v>223434</v>
+        <v>4324234</v>
       </c>
       <c r="F11" t="n">
         <v>232423</v>
@@ -1021,14 +1021,14 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>wqqtrre</t>
+          <t>Funciona</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>23424</v>
+        <v>11111</v>
       </c>
       <c r="E13" t="n">
-        <v>3424234</v>
+        <v>33333</v>
       </c>
       <c r="F13" t="n">
         <v>2342342</v>
@@ -1039,6 +1039,104 @@
       <c r="H13" t="inlineStr">
         <is>
           <t>04/06/2024 04:46</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>El Circulo</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>1112232121312</v>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Dog</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>222222</v>
+      </c>
+      <c r="E14" t="n">
+        <v>111111</v>
+      </c>
+      <c r="F14" t="n">
+        <v>1221</v>
+      </c>
+      <c r="G14" t="b">
+        <v>1</v>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>04/06/2024 06:54</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>The Chronic</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>1123213432133</v>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Aftermath</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>100000</v>
+      </c>
+      <c r="E15" t="n">
+        <v>10000000</v>
+      </c>
+      <c r="F15" t="n">
+        <v>3333</v>
+      </c>
+      <c r="G15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>04/06/2024 07:01</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Perchalsts</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>3423423432432</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>sdffsdf</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>4234234</v>
+      </c>
+      <c r="E16" t="n">
+        <v>234234</v>
+      </c>
+      <c r="F16" t="n">
+        <v>234234</v>
+      </c>
+      <c r="G16" t="b">
+        <v>1</v>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>04/06/2024 07:16</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Se esta terminando de cocinar la ventana de ventas
</commit_message>
<xml_diff>
--- a/registros.xlsx
+++ b/registros.xlsx
@@ -434,7 +434,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -520,6 +520,19 @@
       </c>
       <c r="C5" t="n">
         <v>323234323</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>1000535410</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>pedro</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>3452353234</v>
       </c>
     </row>
   </sheetData>
@@ -598,7 +611,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H16"/>
+  <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -608,7 +621,7 @@
   <cols>
     <col width="13" customWidth="1" min="1" max="1"/>
     <col width="18" customWidth="1" min="2" max="2"/>
-    <col width="11" customWidth="1" min="3" max="3"/>
+    <col width="14" customWidth="1" min="3" max="3"/>
     <col width="23" customWidth="1" min="4" max="4"/>
     <col width="14" customWidth="1" min="5" max="5"/>
     <col width="19" customWidth="1" min="6" max="6"/>
@@ -1112,10 +1125,8 @@
           <t>Perchalsts</t>
         </is>
       </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>3423423432432</t>
-        </is>
+      <c r="B16" t="n">
+        <v>3423423432432</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
@@ -1137,6 +1148,70 @@
       <c r="H16" t="inlineStr">
         <is>
           <t>04/06/2024 07:16</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>DarkElf</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>9292929219191</v>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>oneonoe</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>259000</v>
+      </c>
+      <c r="E17" t="n">
+        <v>400000</v>
+      </c>
+      <c r="F17" t="n">
+        <v>90</v>
+      </c>
+      <c r="G17" t="b">
+        <v>1</v>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>04/06/2024 09:03</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>perro</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>3243242342342</v>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>funcionahpta</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>32323</v>
+      </c>
+      <c r="E18" t="n">
+        <v>6547454</v>
+      </c>
+      <c r="F18" t="n">
+        <v>4242342</v>
+      </c>
+      <c r="G18" t="b">
+        <v>1</v>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>04/06/2024 09:06</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
fetching current github repository
</commit_message>
<xml_diff>
--- a/registros.xlsx
+++ b/registros.xlsx
@@ -434,7 +434,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -507,19 +507,6 @@
       </c>
       <c r="C4" t="n">
         <v>2342345467</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>1222323423</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Validasras</t>
-        </is>
-      </c>
-      <c r="C5" t="n">
-        <v>323234323</v>
       </c>
     </row>
   </sheetData>
@@ -1112,10 +1099,8 @@
           <t>Perchalsts</t>
         </is>
       </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>3423423432432</t>
-        </is>
+      <c r="B16" t="n">
+        <v>3423423432432</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
@@ -1348,7 +1333,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1358,7 +1343,7 @@
   <cols>
     <col width="13" customWidth="1" min="1" max="1"/>
     <col width="17" customWidth="1" min="2" max="2"/>
-    <col width="7" customWidth="1" min="3" max="3"/>
+    <col width="11" customWidth="1" min="3" max="3"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1376,6 +1361,19 @@
         <is>
           <t>Costo</t>
         </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>213123123</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>asdsadas</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>213123123</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Cambios en Administracion de usuarios.ui
</commit_message>
<xml_diff>
--- a/registros.xlsx
+++ b/registros.xlsx
@@ -434,7 +434,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -472,32 +472,41 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
+        <v>43870330</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Ester</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>3105206465</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>71722939</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Carlos</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>3022350912</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
         <v>1013337950</v>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="B4" t="inlineStr">
         <is>
           <t>Alejandro</t>
         </is>
       </c>
-      <c r="C2" t="n">
+      <c r="C4" t="n">
         <v>3015305600</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>71722939</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Carlos</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>3206149912</t>
-        </is>
       </c>
     </row>
   </sheetData>
@@ -576,7 +585,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -586,7 +595,7 @@
   <cols>
     <col width="12" customWidth="1" min="1" max="1"/>
     <col width="18" customWidth="1" min="2" max="2"/>
-    <col width="12" customWidth="1" min="3" max="3"/>
+    <col width="8" customWidth="1" min="3" max="3"/>
     <col width="23" customWidth="1" min="4" max="4"/>
     <col width="14" customWidth="1" min="5" max="5"/>
     <col width="19" customWidth="1" min="6" max="6"/>
@@ -775,14 +784,14 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Margartira</t>
+          <t>Exito</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>2000</v>
+        <v>30000</v>
       </c>
       <c r="E6" t="n">
-        <v>5000</v>
+        <v>20000</v>
       </c>
       <c r="F6" t="n">
         <v>324</v>
@@ -807,14 +816,14 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Tostada</t>
+          <t>Zenu</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>2000</v>
+        <v>1500</v>
       </c>
       <c r="E7" t="n">
-        <v>4000</v>
+        <v>3500</v>
       </c>
       <c r="F7" t="n">
         <v>20</v>
@@ -825,6 +834,102 @@
       <c r="H7" t="inlineStr">
         <is>
           <t>04/06/2024 14:40</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Zapatos</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>7702003141516</v>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Adidas</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>20</v>
+      </c>
+      <c r="E8" t="n">
+        <v>30</v>
+      </c>
+      <c r="F8" t="n">
+        <v>20</v>
+      </c>
+      <c r="G8" t="b">
+        <v>1</v>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>04/06/2024 16:19</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Camiseta</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>7702034121618</v>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Rifle</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>10</v>
+      </c>
+      <c r="E9" t="n">
+        <v>50</v>
+      </c>
+      <c r="F9" t="n">
+        <v>15</v>
+      </c>
+      <c r="G9" t="b">
+        <v>1</v>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>04/06/2024 17:03</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Gorra</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>7703001565152</v>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Calvin</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>40</v>
+      </c>
+      <c r="E10" t="n">
+        <v>70</v>
+      </c>
+      <c r="F10" t="n">
+        <v>20</v>
+      </c>
+      <c r="G10" t="b">
+        <v>1</v>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>04/06/2024 17:26</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
end day commit, modificacion ventana reportes
</commit_message>
<xml_diff>
--- a/registros.xlsx
+++ b/registros.xlsx
@@ -1141,7 +1141,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1149,7 +1149,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="13" customWidth="1" min="1" max="1"/>
+    <col width="14" customWidth="1" min="1" max="1"/>
     <col width="17" customWidth="1" min="2" max="2"/>
     <col width="7" customWidth="1" min="3" max="3"/>
   </cols>
@@ -1169,6 +1169,19 @@
         <is>
           <t>Costo</t>
         </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>123231232321</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Canalo</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>30000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Se corrige crasheo ULTIMO COMMIT AHORA SI
</commit_message>
<xml_diff>
--- a/registros.xlsx
+++ b/registros.xlsx
@@ -434,7 +434,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -442,9 +442,9 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="8" customWidth="1" min="1" max="1"/>
+    <col width="10" customWidth="1" min="1" max="1"/>
     <col width="8" customWidth="1" min="2" max="2"/>
-    <col width="10" customWidth="1" min="3" max="3"/>
+    <col width="11" customWidth="1" min="3" max="3"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -462,6 +462,19 @@
         <is>
           <t>Telefono</t>
         </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>71722939</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Alan</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>838383838</v>
       </c>
     </row>
   </sheetData>
@@ -540,7 +553,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -555,7 +568,7 @@
     <col width="14" customWidth="1" min="5" max="5"/>
     <col width="19" customWidth="1" min="6" max="6"/>
     <col width="21" customWidth="1" min="7" max="7"/>
-    <col width="7" customWidth="1" min="8" max="8"/>
+    <col width="12" customWidth="1" min="8" max="8"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -597,6 +610,38 @@
       <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Fecha</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Pestanina</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>7701001656464</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Vogue</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>70</v>
+      </c>
+      <c r="E2" t="n">
+        <v>100</v>
+      </c>
+      <c r="F2" t="n">
+        <v>80</v>
+      </c>
+      <c r="G2" t="b">
+        <v>1</v>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>2024-06-06</t>
         </is>
       </c>
     </row>
@@ -676,7 +721,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -685,12 +730,12 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="10" customWidth="1" min="1" max="1"/>
-    <col width="8" customWidth="1" min="2" max="2"/>
-    <col width="9" customWidth="1" min="3" max="3"/>
-    <col width="10" customWidth="1" min="4" max="4"/>
-    <col width="7" customWidth="1" min="5" max="5"/>
+    <col width="10" customWidth="1" min="2" max="2"/>
+    <col width="39" customWidth="1" min="3" max="3"/>
+    <col width="50" customWidth="1" min="4" max="4"/>
+    <col width="18" customWidth="1" min="5" max="5"/>
     <col width="10" customWidth="1" min="6" max="6"/>
-    <col width="10" customWidth="1" min="7" max="7"/>
+    <col width="43" customWidth="1" min="7" max="7"/>
     <col width="15" customWidth="1" min="8" max="8"/>
   </cols>
   <sheetData>
@@ -734,6 +779,296 @@
         <is>
           <t>ID_MetodoPago</t>
         </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Series([], Name: Nombre Servicio, dtype: object)</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>06/06/2024 15:12</t>
+        </is>
+      </c>
+      <c r="F2" t="n">
+        <v>1</v>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>0    897
+Name: Costo, dtype: int64</t>
+        </is>
+      </c>
+      <c r="H2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>0</v>
+      </c>
+      <c r="B3" t="n">
+        <v>71722939</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>0    Alan
+Name: Nombre, dtype: object</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Series([], Name: Nombre Servicio, dtype: object)</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>06/06/2024 15:14</t>
+        </is>
+      </c>
+      <c r="F3" t="n">
+        <v>1</v>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>0    897
+Name: Costo, dtype: int64</t>
+        </is>
+      </c>
+      <c r="H3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>836</v>
+      </c>
+      <c r="B4" t="n">
+        <v>71722939</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>0    Alan
+Name: Nombre, dtype: object</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>0    Pestanina
+Name: Referencia, dtype: object</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>06/06/2024 15:18</t>
+        </is>
+      </c>
+      <c r="F4" t="n">
+        <v>3</v>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>0    300
+Name: Precio venta, dtype: int64</t>
+        </is>
+      </c>
+      <c r="H4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>0</v>
+      </c>
+      <c r="B5" t="n">
+        <v>71722939</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>0    Alan
+Name: Nombre, dtype: object</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Series([], Name: Nombre Servicio, dtype: object)</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>06/06/2024 15:18</t>
+        </is>
+      </c>
+      <c r="F5" t="n">
+        <v>1</v>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>0    897
+Name: Costo, dtype: int64</t>
+        </is>
+      </c>
+      <c r="H5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>48</v>
+      </c>
+      <c r="B6" t="n">
+        <v>71722939</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>0    Alan
+Name: Nombre, dtype: object</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>0    Pestanina
+Name: Referencia, dtype: object</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>06/06/2024 15:21</t>
+        </is>
+      </c>
+      <c r="F6" t="n">
+        <v>2</v>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>0    200
+Name: Precio venta, dtype: int64</t>
+        </is>
+      </c>
+      <c r="H6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>0</v>
+      </c>
+      <c r="B7" t="n">
+        <v>71722939</v>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>0    Alan
+Name: Nombre, dtype: object</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Series([], Name: Nombre Servicio, dtype: object)</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>06/06/2024 15:21</t>
+        </is>
+      </c>
+      <c r="F7" t="n">
+        <v>3</v>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>0    2691
+Name: Costo, dtype: int64</t>
+        </is>
+      </c>
+      <c r="H7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>409</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>71722939</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>0    Alan
+Name: Nombre, dtype: object</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>0    Pestanina
+Name: Referencia, dtype: object</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>06/06/2024 15:23</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>0    300
+Name: Precio venta, dtype: int64</t>
+        </is>
+      </c>
+      <c r="H8" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>0</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>71722939</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>0    Alan
+Name: Nombre, dtype: object</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Series([], Name: Nombre Servicio, dtype: object)</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>06/06/2024 15:23</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>0    2691
+Name: Costo, dtype: int64</t>
+        </is>
+      </c>
+      <c r="H9" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -818,7 +1153,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -846,6 +1181,19 @@
         <is>
           <t>Costo</t>
         </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>7272737373</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Maquillaje</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>897</v>
       </c>
     </row>
   </sheetData>

</xml_diff>